<commit_message>
add a script to send sample messages
</commit_message>
<xml_diff>
--- a/test/fixtures/sample.xlsx
+++ b/test/fixtures/sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -121,7 +121,7 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>0775090901</t>
+    <t>+256790513253</t>
   </si>
   <si>
     <t>LIB-MAG-004</t>
@@ -152,9 +152,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="MMM\ DD"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -242,7 +243,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -269,6 +270,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -286,13 +291,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -521,14 +526,14 @@
       </c>
       <c r="J7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -553,7 +558,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -596,13 +601,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C11:C12 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -632,13 +637,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C11:C12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
make sure response of sending includes status and phone numbers etc.
</commit_message>
<xml_diff>
--- a/test/fixtures/sample.xlsx
+++ b/test/fixtures/sample.xlsx
@@ -121,7 +121,7 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>+256790513253</t>
+    <t>12345</t>
   </si>
   <si>
     <t>LIB-MAG-004</t>
@@ -297,7 +297,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11:C12"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -607,7 +607,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C11:C12 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -643,7 +643,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C11:C12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>